<commit_message>
updated functions to match MATLAB outputs for muscle data when run from the test script
</commit_message>
<xml_diff>
--- a/Master_AnatomicalData.xlsx
+++ b/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DD421B-474D-4926-9D2C-A8894C308A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D0C629-939C-49F1-BCF5-4827EB941723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="2280" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="7" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="405" yWindow="2280" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -910,9 +910,6 @@
     <t>brachial_muscle_mass</t>
   </si>
   <si>
-    <t>antbrachial_muscle_mass</t>
-  </si>
-  <si>
     <t>manus_muscle_mass</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>bone</t>
+  </si>
+  <si>
+    <t>antebrachial_muscle_mass</t>
   </si>
 </sst>
 </file>
@@ -11693,11 +11693,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBCFE0-47B2-4031-92B0-C1E328A3FA99}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11744,22 +11744,22 @@
         <v>284</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>267</v>
@@ -11813,6 +11813,15 @@
       <c r="E2">
         <f>D2*(6.7-1)</f>
         <v>1.5105000000000001E-4</v>
+      </c>
+      <c r="F2">
+        <v>9.9351793580869999E-3</v>
+      </c>
+      <c r="G2">
+        <v>5.7127281309000003E-3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.09286972938955E-4</v>
       </c>
       <c r="I2">
         <f>(49.33*10^-3-(SUM(Feathers!J2:J32))/1000)/2</f>
@@ -11913,28 +11922,28 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" t="s">
         <v>291</v>
-      </c>
-      <c r="D1" t="s">
-        <v>292</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G1" t="s">
         <v>293</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>294</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>295</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>296</v>
-      </c>
-      <c r="J1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13072,7 +13081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B73562-5146-43F5-B742-9562EED8ED07}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -13091,19 +13100,19 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
         <v>298</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>299</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>300</v>
-      </c>
-      <c r="F1" t="s">
-        <v>301</v>
       </c>
       <c r="G1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
updated the skin calculations
</commit_message>
<xml_diff>
--- a/Master_AnatomicalData.xlsx
+++ b/Master_AnatomicalData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D0C629-939C-49F1-BCF5-4827EB941723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF118B8E-3528-4C84-B5E3-21D64DB2EA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="2280" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
@@ -913,9 +913,6 @@
     <t>manus_muscle_mass</t>
   </si>
   <si>
-    <t>propatagiale_skin_mas</t>
-  </si>
-  <si>
     <t>manus_skin_mass</t>
   </si>
   <si>
@@ -962,6 +959,9 @@
   </si>
   <si>
     <t>antebrachial_muscle_mass</t>
+  </si>
+  <si>
+    <t>propatagiale_skin_mass</t>
   </si>
 </sst>
 </file>
@@ -11697,7 +11697,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11744,22 +11744,22 @@
         <v>284</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>285</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>267</v>
@@ -11824,12 +11824,10 @@
         <v>1.09286972938955E-4</v>
       </c>
       <c r="I2">
-        <f>(49.33*10^-3-(SUM(Feathers!J2:J32))/1000)/2</f>
-        <v>1.8748149999999998E-2</v>
+        <v>3.5262422312465E-2</v>
       </c>
       <c r="J2">
-        <f>(49.33*10^-3-(SUM(Feathers!J2:J32))/1000)/2</f>
-        <v>1.8748149999999998E-2</v>
+        <v>2.2338776875349999E-3</v>
       </c>
       <c r="W2" t="s">
         <v>49</v>
@@ -11922,28 +11920,28 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" t="s">
         <v>290</v>
-      </c>
-      <c r="D1" t="s">
-        <v>291</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1" t="s">
         <v>292</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>293</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>294</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>295</v>
-      </c>
-      <c r="J1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13100,19 +13098,19 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" t="s">
         <v>297</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>298</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>299</v>
-      </c>
-      <c r="F1" t="s">
-        <v>300</v>
       </c>
       <c r="G1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
created function to calculate the feather orientation (uses linear interpolation); verified that feather mass properties agreed with MATLAB
</commit_message>
<xml_diff>
--- a/Master_AnatomicalData.xlsx
+++ b/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF118B8E-3528-4C84-B5E3-21D64DB2EA53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979A4FDF-3BB1-4839-8EE0-F317915EAB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="2280" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="33300" yWindow="2055" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="6" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -937,12 +937,6 @@
     <t>w_vd</t>
   </si>
   <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Mass</t>
-  </si>
-  <si>
     <t>bone_mass</t>
   </si>
   <si>
@@ -962,6 +956,12 @@
   </si>
   <si>
     <t>propatagiale_skin_mass</t>
+  </si>
+  <si>
+    <t>l_f</t>
+  </si>
+  <si>
+    <t>m_f</t>
   </si>
 </sst>
 </file>
@@ -11693,7 +11693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBCFE0-47B2-4031-92B0-C1E328A3FA99}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -11744,13 +11744,13 @@
         <v>284</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>285</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>286</v>
@@ -11899,8 +11899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69E9DF-4385-4F68-B3FA-768F27E5E0EC}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11909,7 +11909,7 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -11938,10 +11938,10 @@
         <v>293</v>
       </c>
       <c r="I1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="J1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13098,19 +13098,19 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
         <v>296</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>297</v>
-      </c>
-      <c r="E1" t="s">
-        <v>298</v>
-      </c>
-      <c r="F1" t="s">
-        <v>299</v>
       </c>
       <c r="G1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
updated to store all data for wing mass properties
</commit_message>
<xml_diff>
--- a/Master_AnatomicalData.xlsx
+++ b/Master_AnatomicalData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979A4FDF-3BB1-4839-8EE0-F317915EAB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E89F270-AA11-4BA3-B2A9-060E340EA221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33300" yWindow="2055" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="6" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
@@ -1109,7 +1109,7 @@
       <sheetName val="Final"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="F2">
@@ -5768,8 +5768,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11900,7 +11900,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>